<commit_message>
Uploaded 06-May-2021 13:11:50 {/src/main/resources/com/wakandaspace/drools_price_model/premiumCalculation.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/wakandaspace/drools_price_model/premiumCalculation.xlsx
+++ b/src/main/resources/com/wakandaspace/drools_price_model/premiumCalculation.xlsx
@@ -651,8 +651,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K935"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10:G11"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -782,7 +782,9 @@
     </row>
     <row r="8" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="14"/>
-      <c r="B8" s="15"/>
+      <c r="B8" s="15">
+        <v>16</v>
+      </c>
       <c r="C8" s="19" t="s">
         <v>9</v>
       </c>
@@ -797,7 +799,9 @@
     </row>
     <row r="9" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="14"/>
-      <c r="B9" s="15"/>
+      <c r="B9" s="15">
+        <v>16</v>
+      </c>
       <c r="C9" s="19" t="s">
         <v>10</v>
       </c>
@@ -812,7 +816,9 @@
     </row>
     <row r="10" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="14"/>
-      <c r="B10" s="15"/>
+      <c r="B10" s="15">
+        <v>16</v>
+      </c>
       <c r="C10" s="19"/>
       <c r="D10" s="19"/>
       <c r="E10" s="19" t="s">

</xml_diff>

<commit_message>
Uploaded 06-May-2021 13:15:15 {/src/main/resources/com/wakandaspace/drools_price_model/premiumCalculation.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/wakandaspace/drools_price_model/premiumCalculation.xlsx
+++ b/src/main/resources/com/wakandaspace/drools_price_model/premiumCalculation.xlsx
@@ -649,10 +649,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K935"/>
+  <dimension ref="A1:K934"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -751,34 +751,42 @@
       </c>
     </row>
     <row r="6" spans="1:11" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-    </row>
-    <row r="7" spans="1:11" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="11" t="s">
+      <c r="A6" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B6" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C6" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D6" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E6" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="13" t="s">
+      <c r="F6" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="13"/>
+      <c r="G6" s="13"/>
+    </row>
+    <row r="7" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="A7" s="14"/>
+      <c r="B7" s="15">
+        <v>16</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="19"/>
+      <c r="F7" s="20">
+        <v>0.91200000000000003</v>
+      </c>
+      <c r="G7" s="20"/>
     </row>
     <row r="8" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="14"/>
@@ -786,14 +794,14 @@
         <v>16</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D8" s="19" t="s">
         <v>12</v>
       </c>
       <c r="E8" s="19"/>
       <c r="F8" s="20">
-        <v>0.91200000000000003</v>
+        <v>1</v>
       </c>
       <c r="G8" s="20"/>
     </row>
@@ -802,23 +810,19 @@
       <c r="B9" s="15">
         <v>16</v>
       </c>
-      <c r="C9" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="19" t="s">
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="19"/>
-      <c r="F9" s="20">
-        <v>1</v>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20" t="s">
+        <v>12</v>
       </c>
-      <c r="G9" s="20"/>
     </row>
     <row r="10" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="14"/>
-      <c r="B10" s="15">
-        <v>16</v>
-      </c>
+      <c r="B10" s="15"/>
       <c r="C10" s="19"/>
       <c r="D10" s="19"/>
       <c r="E10" s="19" t="s">
@@ -834,13 +838,9 @@
       <c r="B11" s="15"/>
       <c r="C11" s="19"/>
       <c r="D11" s="19"/>
-      <c r="E11" s="19" t="s">
-        <v>12</v>
-      </c>
+      <c r="E11" s="19"/>
       <c r="F11" s="20"/>
-      <c r="G11" s="20" t="s">
-        <v>12</v>
-      </c>
+      <c r="G11" s="20"/>
     </row>
     <row r="12" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="14"/>
@@ -905,14 +905,14 @@
       <c r="F18" s="20"/>
       <c r="G18" s="20"/>
     </row>
-    <row r="19" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="14"/>
       <c r="B19" s="15"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="20"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="14"/>
@@ -9148,15 +9148,6 @@
       <c r="E934" s="14"/>
       <c r="F934" s="16"/>
       <c r="G934" s="16"/>
-    </row>
-    <row r="935" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A935" s="14"/>
-      <c r="B935" s="15"/>
-      <c r="C935" s="14"/>
-      <c r="D935" s="14"/>
-      <c r="E935" s="14"/>
-      <c r="F935" s="16"/>
-      <c r="G935" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Uploaded 06-May-2021 13:20:32 {/src/main/resources/com/wakandaspace/drools_price_model/premiumCalculation.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/wakandaspace/drools_price_model/premiumCalculation.xlsx
+++ b/src/main/resources/com/wakandaspace/drools_price_model/premiumCalculation.xlsx
@@ -271,14 +271,14 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="10" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -651,8 +651,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K934"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -674,24 +674,24 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
       <c r="G1" s="21"/>
     </row>
     <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
       <c r="G2" s="21"/>
       <c r="K2" s="3"/>
     </row>
@@ -725,10 +725,10 @@
       <c r="C4" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="23" t="s">
+      <c r="D4" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="24"/>
+      <c r="E4" s="23"/>
       <c r="F4" s="8"/>
       <c r="G4" s="8"/>
       <c r="K4" s="3"/>
@@ -9152,10 +9152,9 @@
       <c r="G934" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="2">
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="A2:F2"/>
-    <mergeCell ref="D4:E4"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" r:id="rId1"/>

</xml_diff>

<commit_message>
Uploaded 06-May-2021 13:23:30 {/src/main/resources/com/wakandaspace/drools_price_model/premiumCalculation.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/wakandaspace/drools_price_model/premiumCalculation.xlsx
+++ b/src/main/resources/com/wakandaspace/drools_price_model/premiumCalculation.xlsx
@@ -78,7 +78,7 @@
     <t>$sumFinalFactor :Double() from accumulate (Benefit(calculationR : calculationResult), sum(calculationR))</t>
   </si>
   <si>
-    <t>$plan.setIndividualPremiumResult($plan.getIndividualPremiumResult()*$sumFinalFactor)</t>
+    <t>$plan.setIndividualPremiumResult($plan.getIndividualPremiumResult()*$sumFinalFactor);</t>
   </si>
 </sst>
 </file>
@@ -651,8 +651,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K934"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" outlineLevelRow="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Uploaded 06-May-2021 14:43:45 {/src/main/resources/com/wakandaspace/drools_price_model/premiumCalculation.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/wakandaspace/drools_price_model/premiumCalculation.xlsx
+++ b/src/main/resources/com/wakandaspace/drools_price_model/premiumCalculation.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="19">
   <si>
     <t>RuleSet</t>
   </si>
@@ -665,8 +665,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M934"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -726,8 +726,12 @@
       <c r="D3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
+      <c r="E3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>4</v>
+      </c>
       <c r="G3" s="6" t="s">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
Uploaded 06-May-2021 14:48:23 {/src/main/resources/com/wakandaspace/drools_price_model/premiumCalculation.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/wakandaspace/drools_price_model/premiumCalculation.xlsx
+++ b/src/main/resources/com/wakandaspace/drools_price_model/premiumCalculation.xlsx
@@ -665,8 +665,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M934"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -881,9 +881,7 @@
     </row>
     <row r="11" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="14"/>
-      <c r="B11" s="15">
-        <v>16</v>
-      </c>
+      <c r="B11" s="15"/>
       <c r="C11" s="19"/>
       <c r="D11" s="19"/>
       <c r="E11" s="19"/>
@@ -894,9 +892,7 @@
     </row>
     <row r="12" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="14"/>
-      <c r="B12" s="15">
-        <v>16</v>
-      </c>
+      <c r="B12" s="15"/>
       <c r="C12" s="19"/>
       <c r="D12" s="19"/>
       <c r="E12" s="19"/>

</xml_diff>

<commit_message>
Uploaded 06-May-2021 14:54:25 {/src/main/resources/com/wakandaspace/drools_price_model/premiumCalculation.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/wakandaspace/drools_price_model/premiumCalculation.xlsx
+++ b/src/main/resources/com/wakandaspace/drools_price_model/premiumCalculation.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="23">
   <si>
     <t>RuleSet</t>
   </si>
@@ -40,9 +40,6 @@
   </si>
   <si>
     <t>factor</t>
-  </si>
-  <si>
-    <t>$plan:Plan</t>
   </si>
   <si>
     <t>getPreAuthorizationRequired().equals("$paramater")</t>
@@ -76,6 +73,21 @@
   </si>
   <si>
     <t>$plan.setIndividualPremiumResult(($plan.getIndividualPremiumResult()/$expense.getLossRatioTarget())*12);</t>
+  </si>
+  <si>
+    <t>preauthoriationFactor1</t>
+  </si>
+  <si>
+    <t>preauthoriationFactor2</t>
+  </si>
+  <si>
+    <t>premiumCalculation1</t>
+  </si>
+  <si>
+    <t>premiumCalculation2</t>
+  </si>
+  <si>
+    <t>$plan:Plan()</t>
   </si>
 </sst>
 </file>
@@ -665,8 +677,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M934"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -701,7 +713,7 @@
     </row>
     <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="23" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B2" s="23"/>
       <c r="C2" s="23"/>
@@ -747,11 +759,11 @@
       <c r="A4" s="7"/>
       <c r="B4" s="7"/>
       <c r="C4" s="24" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="D4" s="25"/>
       <c r="E4" s="26" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F4" s="22"/>
       <c r="G4" s="8"/>
@@ -763,21 +775,21 @@
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
       <c r="F5" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="H5" s="10" t="s">
-        <v>16</v>
-      </c>
       <c r="I5" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.2">
@@ -788,7 +800,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D6" s="12"/>
       <c r="E6" s="12"/>
@@ -800,12 +812,14 @@
       <c r="I6" s="13"/>
     </row>
     <row r="7" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A7" s="14"/>
+      <c r="A7" s="14" t="s">
+        <v>18</v>
+      </c>
       <c r="B7" s="15">
         <v>16</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D7" s="19"/>
       <c r="E7" s="19"/>
@@ -817,12 +831,14 @@
       <c r="I7" s="20"/>
     </row>
     <row r="8" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A8" s="14"/>
+      <c r="A8" s="14" t="s">
+        <v>19</v>
+      </c>
       <c r="B8" s="15">
         <v>16</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D8" s="19"/>
       <c r="E8" s="19"/>
@@ -834,49 +850,53 @@
       <c r="I8" s="20"/>
     </row>
     <row r="9" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A9" s="14"/>
+      <c r="A9" s="14" t="s">
+        <v>20</v>
+      </c>
       <c r="B9" s="15">
         <v>16</v>
       </c>
       <c r="C9" s="19"/>
       <c r="D9" s="19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E9" s="19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G9" s="20"/>
       <c r="H9" s="20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I9" s="20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A10" s="14"/>
+      <c r="A10" s="14" t="s">
+        <v>21</v>
+      </c>
       <c r="B10" s="15">
         <v>16</v>
       </c>
       <c r="C10" s="19"/>
       <c r="D10" s="19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E10" s="19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F10" s="19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G10" s="20"/>
       <c r="H10" s="20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I10" s="20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Uploaded 06-May-2021 14:59:56 {/src/main/resources/com/wakandaspace/drools_price_model/premiumCalculation.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/wakandaspace/drools_price_model/premiumCalculation.xlsx
+++ b/src/main/resources/com/wakandaspace/drools_price_model/premiumCalculation.xlsx
@@ -63,9 +63,6 @@
     <t>RuleTable premiumCalculation</t>
   </si>
   <si>
-    <t>$plan.setIndividualPremiumResult($param)</t>
-  </si>
-  <si>
     <t>$sumFinalFactor :Double() from accumulate (Benefit(calculationR : calculationResult), sum(calculationR))</t>
   </si>
   <si>
@@ -88,6 +85,9 @@
   </si>
   <si>
     <t>premiumCalculation2</t>
+  </si>
+  <si>
+    <t>$plan.setIndividualPremiumResult($param);</t>
   </si>
 </sst>
 </file>
@@ -674,8 +674,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M934"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E4" s="25" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F4" s="22"/>
       <c r="G4" s="8"/>
@@ -779,16 +779,16 @@
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
       <c r="F5" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="H5" s="10" t="s">
-        <v>16</v>
-      </c>
       <c r="I5" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.2">
@@ -812,7 +812,7 @@
     </row>
     <row r="7" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B7" s="15">
         <v>16</v>
@@ -831,7 +831,7 @@
     </row>
     <row r="8" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B8" s="15">
         <v>16</v>
@@ -850,7 +850,7 @@
     </row>
     <row r="9" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B9" s="15">
         <v>16</v>
@@ -875,7 +875,7 @@
     </row>
     <row r="10" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B10" s="15">
         <v>16</v>

</xml_diff>

<commit_message>
Uploaded 06-May-2021 15:01:51 {/src/main/resources/com/wakandaspace/drools_price_model/premiumCalculation.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/wakandaspace/drools_price_model/premiumCalculation.xlsx
+++ b/src/main/resources/com/wakandaspace/drools_price_model/premiumCalculation.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="22">
   <si>
     <t>RuleSet</t>
   </si>
@@ -81,13 +81,10 @@
     <t>preauthoriationFactor2</t>
   </si>
   <si>
-    <t>premiumCalculation1</t>
+    <t>$plan.setIndividualPremiumResult($param);</t>
   </si>
   <si>
-    <t>premiumCalculation2</t>
-  </si>
-  <si>
-    <t>$plan.setIndividualPremiumResult($param);</t>
+    <t>premiumCalculation</t>
   </si>
 </sst>
 </file>
@@ -672,10 +669,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M934"/>
+  <dimension ref="A1:M933"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -782,7 +779,7 @@
         <v>14</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H5" s="10" t="s">
         <v>15</v>
@@ -850,7 +847,7 @@
     </row>
     <row r="9" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B9" s="15">
         <v>16</v>
@@ -874,29 +871,15 @@
       </c>
     </row>
     <row r="10" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="15">
-        <v>16</v>
-      </c>
+      <c r="A10" s="14"/>
+      <c r="B10" s="15"/>
       <c r="C10" s="19"/>
-      <c r="D10" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" s="19" t="s">
-        <v>11</v>
-      </c>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
       <c r="G10" s="20"/>
-      <c r="H10" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="I10" s="20" t="s">
-        <v>11</v>
-      </c>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20"/>
     </row>
     <row r="11" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="14"/>
@@ -975,16 +958,16 @@
       <c r="H17" s="20"/>
       <c r="I17" s="20"/>
     </row>
-    <row r="18" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="14"/>
       <c r="B18" s="15"/>
-      <c r="C18" s="19"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="20"/>
-      <c r="H18" s="20"/>
-      <c r="I18" s="20"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="16"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="14"/>
@@ -11050,17 +11033,6 @@
       <c r="G933" s="16"/>
       <c r="H933" s="16"/>
       <c r="I933" s="16"/>
-    </row>
-    <row r="934" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A934" s="14"/>
-      <c r="B934" s="15"/>
-      <c r="C934" s="14"/>
-      <c r="D934" s="14"/>
-      <c r="E934" s="14"/>
-      <c r="F934" s="14"/>
-      <c r="G934" s="16"/>
-      <c r="H934" s="16"/>
-      <c r="I934" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Uploaded 06-May-2021 15:03:57 {/src/main/resources/com/wakandaspace/drools_price_model/premiumCalculation.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/wakandaspace/drools_price_model/premiumCalculation.xlsx
+++ b/src/main/resources/com/wakandaspace/drools_price_model/premiumCalculation.xlsx
@@ -48,12 +48,6 @@
     <t>getPreAuthorizationRequired().equals("$paramater")</t>
   </si>
   <si>
-    <t>YES</t>
-  </si>
-  <si>
-    <t>NO</t>
-  </si>
-  <si>
     <t>true</t>
   </si>
   <si>
@@ -85,6 +79,12 @@
   </si>
   <si>
     <t>premiumCalculation</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>no</t>
   </si>
 </sst>
 </file>
@@ -672,7 +672,7 @@
   <dimension ref="A1:M933"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -707,7 +707,7 @@
     </row>
     <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B2" s="24"/>
       <c r="C2" s="24"/>
@@ -759,7 +759,7 @@
         <v>7</v>
       </c>
       <c r="E4" s="25" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F4" s="22"/>
       <c r="G4" s="8"/>
@@ -776,16 +776,16 @@
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
       <c r="F5" s="9" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I5" s="10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.2">
@@ -796,7 +796,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D6" s="12"/>
       <c r="E6" s="12"/>
@@ -809,13 +809,13 @@
     </row>
     <row r="7" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B7" s="15">
         <v>16</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="D7" s="19"/>
       <c r="E7" s="19"/>
@@ -828,13 +828,13 @@
     </row>
     <row r="8" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B8" s="15">
         <v>16</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="D8" s="19"/>
       <c r="E8" s="19"/>
@@ -847,27 +847,27 @@
     </row>
     <row r="9" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B9" s="15">
         <v>16</v>
       </c>
       <c r="C9" s="19"/>
       <c r="D9" s="19" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E9" s="19" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G9" s="20"/>
       <c r="H9" s="20" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="I9" s="20" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Uploaded 06-May-2021 15:05:37 {/src/main/resources/com/wakandaspace/drools_price_model/premiumCalculation.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/wakandaspace/drools_price_model/premiumCalculation.xlsx
+++ b/src/main/resources/com/wakandaspace/drools_price_model/premiumCalculation.xlsx
@@ -45,9 +45,6 @@
     <t>$plan:Plan</t>
   </si>
   <si>
-    <t>getPreAuthorizationRequired().equals("$paramater")</t>
-  </si>
-  <si>
     <t>true</t>
   </si>
   <si>
@@ -85,6 +82,9 @@
   </si>
   <si>
     <t>no</t>
+  </si>
+  <si>
+    <t>getPreAuthorizationRequired().equals("$param")</t>
   </si>
 </sst>
 </file>
@@ -671,8 +671,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M933"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -707,7 +707,7 @@
     </row>
     <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" s="24"/>
       <c r="C2" s="24"/>
@@ -759,7 +759,7 @@
         <v>7</v>
       </c>
       <c r="E4" s="25" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F4" s="22"/>
       <c r="G4" s="8"/>
@@ -771,21 +771,21 @@
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="9" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
       <c r="F5" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="H5" s="10" t="s">
-        <v>13</v>
-      </c>
       <c r="I5" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.2">
@@ -796,7 +796,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D6" s="12"/>
       <c r="E6" s="12"/>
@@ -809,13 +809,13 @@
     </row>
     <row r="7" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" s="15">
         <v>16</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D7" s="19"/>
       <c r="E7" s="19"/>
@@ -828,13 +828,13 @@
     </row>
     <row r="8" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" s="15">
         <v>16</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D8" s="19"/>
       <c r="E8" s="19"/>
@@ -847,27 +847,27 @@
     </row>
     <row r="9" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B9" s="15">
         <v>16</v>
       </c>
       <c r="C9" s="19"/>
       <c r="D9" s="19" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E9" s="19" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G9" s="20"/>
       <c r="H9" s="20" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I9" s="20" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Uploaded 06-May-2021 15:06:26 {/src/main/resources/com/wakandaspace/drools_price_model/premiumCalculation.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/wakandaspace/drools_price_model/premiumCalculation.xlsx
+++ b/src/main/resources/com/wakandaspace/drools_price_model/premiumCalculation.xlsx
@@ -45,6 +45,12 @@
     <t>$plan:Plan</t>
   </si>
   <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
     <t>true</t>
   </si>
   <si>
@@ -76,12 +82,6 @@
   </si>
   <si>
     <t>premiumCalculation</t>
-  </si>
-  <si>
-    <t>yes</t>
-  </si>
-  <si>
-    <t>no</t>
   </si>
   <si>
     <t>getPreAuthorizationRequired().equals("$param")</t>
@@ -672,7 +672,7 @@
   <dimension ref="A1:M933"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -707,7 +707,7 @@
     </row>
     <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B2" s="24"/>
       <c r="C2" s="24"/>
@@ -759,7 +759,7 @@
         <v>7</v>
       </c>
       <c r="E4" s="25" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F4" s="22"/>
       <c r="G4" s="8"/>
@@ -776,16 +776,16 @@
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
       <c r="F5" s="9" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="I5" s="10" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.2">
@@ -796,7 +796,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D6" s="12"/>
       <c r="E6" s="12"/>
@@ -809,13 +809,13 @@
     </row>
     <row r="7" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B7" s="15">
         <v>16</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="D7" s="19"/>
       <c r="E7" s="19"/>
@@ -828,13 +828,13 @@
     </row>
     <row r="8" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B8" s="15">
         <v>16</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D8" s="19"/>
       <c r="E8" s="19"/>
@@ -847,27 +847,27 @@
     </row>
     <row r="9" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B9" s="15">
         <v>16</v>
       </c>
       <c r="C9" s="19"/>
       <c r="D9" s="19" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E9" s="19" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G9" s="20"/>
       <c r="H9" s="20" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="I9" s="20" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Uploaded 06-May-2021 15:10:55 {/src/main/resources/com/wakandaspace/drools_price_model/premiumCalculation.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/wakandaspace/drools_price_model/premiumCalculation.xlsx
+++ b/src/main/resources/com/wakandaspace/drools_price_model/premiumCalculation.xlsx
@@ -672,7 +672,7 @@
   <dimension ref="A1:M933"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -831,7 +831,7 @@
         <v>18</v>
       </c>
       <c r="B8" s="15">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C8" s="19" t="s">
         <v>9</v>
@@ -850,7 +850,7 @@
         <v>20</v>
       </c>
       <c r="B9" s="15">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" s="19"/>
       <c r="D9" s="19" t="s">

</xml_diff>

<commit_message>
Uploaded 06-May-2021 15:13:05 {/src/main/resources/com/wakandaspace/drools_price_model/premiumCalculation.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/wakandaspace/drools_price_model/premiumCalculation.xlsx
+++ b/src/main/resources/com/wakandaspace/drools_price_model/premiumCalculation.xlsx
@@ -672,7 +672,7 @@
   <dimension ref="A1:M933"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -831,7 +831,7 @@
         <v>18</v>
       </c>
       <c r="B8" s="15">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C8" s="19" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Uploaded 06-May-2021 15:17:25 {/src/main/resources/com/wakandaspace/drools_price_model/premiumCalculation.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/wakandaspace/drools_price_model/premiumCalculation.xlsx
+++ b/src/main/resources/com/wakandaspace/drools_price_model/premiumCalculation.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
   <si>
     <t>RuleSet</t>
   </si>
@@ -76,6 +76,9 @@
   </si>
   <si>
     <t>preauthoriationFactor2</t>
+  </si>
+  <si>
+    <t>$plan:Plan()</t>
   </si>
   <si>
     <t>$plan.setIndividualPremiumResult($param);</t>
@@ -672,7 +675,7 @@
   <dimension ref="A1:M933"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -756,7 +759,7 @@
         <v>7</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="E4" s="25" t="s">
         <v>15</v>
@@ -771,7 +774,7 @@
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
@@ -779,7 +782,7 @@
         <v>13</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H5" s="10" t="s">
         <v>14</v>
@@ -847,7 +850,7 @@
     </row>
     <row r="9" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B9" s="15">
         <v>15</v>

</xml_diff>

<commit_message>
Uploaded 10-May-2021 09:44:45 {/src/main/resources/com/wakandaspace/drools_price_model/premiumCalculation.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/wakandaspace/drools_price_model/premiumCalculation.xlsx
+++ b/src/main/resources/com/wakandaspace/drools_price_model/premiumCalculation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="922"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="921"/>
   </bookViews>
   <sheets>
     <sheet name="Tariff" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="27">
   <si>
     <t>RuleSet</t>
   </si>
@@ -88,6 +88,18 @@
   </si>
   <si>
     <t>getPreAuthorizationRequired().equals("$param")</t>
+  </si>
+  <si>
+    <t>plan</t>
+  </si>
+  <si>
+    <t>expense</t>
+  </si>
+  <si>
+    <t>sum Final factor</t>
+  </si>
+  <si>
+    <t>premium result</t>
   </si>
 </sst>
 </file>
@@ -297,11 +309,11 @@
     <xf numFmtId="10" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="10" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -675,7 +687,7 @@
   <dimension ref="A1:M933"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -697,27 +709,27 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
       <c r="H1" s="21"/>
       <c r="I1" s="21"/>
     </row>
     <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
       <c r="H2" s="21"/>
       <c r="I2" s="21"/>
       <c r="M2" s="3"/>
@@ -761,7 +773,7 @@
       <c r="D4" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="25" t="s">
+      <c r="E4" s="24" t="s">
         <v>15</v>
       </c>
       <c r="F4" s="22"/>
@@ -801,14 +813,24 @@
       <c r="C6" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
+      <c r="D6" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>25</v>
+      </c>
       <c r="G6" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
+      <c r="H6" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="I6" s="13" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="7" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">

</xml_diff>

<commit_message>
Uploaded 10-May-2021 10:04:47 {/src/main/resources/com/wakandaspace/drools_price_model/premiumCalculation.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/wakandaspace/drools_price_model/premiumCalculation.xlsx
+++ b/src/main/resources/com/wakandaspace/drools_price_model/premiumCalculation.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="26">
   <si>
     <t>RuleSet</t>
   </si>
@@ -66,9 +66,6 @@
     <t>$plan.setIndividualPremiumResult($plan.getIndividualPremiumResult()*$sumFinalFactor);</t>
   </si>
   <si>
-    <t>$expense: Expense()</t>
-  </si>
-  <si>
     <t>$plan.setIndividualPremiumResult(($plan.getIndividualPremiumResult()/$expense.getLossRatioTarget())*12);</t>
   </si>
   <si>
@@ -78,9 +75,6 @@
     <t>preauthoriationFactor2</t>
   </si>
   <si>
-    <t>$plan:Plan()</t>
-  </si>
-  <si>
     <t>$plan.setIndividualPremiumResult($param);</t>
   </si>
   <si>
@@ -100,6 +94,9 @@
   </si>
   <si>
     <t>premium result</t>
+  </si>
+  <si>
+    <t>$expense: Expense</t>
   </si>
 </sst>
 </file>
@@ -684,7 +681,7 @@
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -768,10 +765,10 @@
         <v>7</v>
       </c>
       <c r="D4" s="22" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="E4" s="23" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="8"/>
@@ -783,21 +780,25 @@
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
+        <v>20</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>10</v>
+      </c>
       <c r="F5" s="9" t="s">
         <v>13</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H5" s="10" t="s">
         <v>14</v>
       </c>
       <c r="I5" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.2">
@@ -811,27 +812,27 @@
         <v>11</v>
       </c>
       <c r="D6" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="12" t="s">
         <v>23</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="F6" s="12" t="s">
-        <v>25</v>
       </c>
       <c r="G6" s="13" t="s">
         <v>6</v>
       </c>
       <c r="H6" s="13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="I6" s="13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7" s="15">
         <v>16</v>
@@ -850,7 +851,7 @@
     </row>
     <row r="8" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B8" s="15">
         <v>16</v>
@@ -869,7 +870,7 @@
     </row>
     <row r="9" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B9" s="15">
         <v>15</v>

</xml_diff>

<commit_message>
Uploaded 10-May-2021 10:15:29 {/src/main/resources/com/wakandaspace/drools_price_model/premiumCalculation.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/wakandaspace/drools_price_model/premiumCalculation.xlsx
+++ b/src/main/resources/com/wakandaspace/drools_price_model/premiumCalculation.xlsx
@@ -42,9 +42,6 @@
     <t>factor</t>
   </si>
   <si>
-    <t>$plan:Plan</t>
-  </si>
-  <si>
     <t>YES</t>
   </si>
   <si>
@@ -97,6 +94,9 @@
   </si>
   <si>
     <t>$expense: Expense</t>
+  </si>
+  <si>
+    <t>$plan: Plan</t>
   </si>
 </sst>
 </file>
@@ -681,7 +681,7 @@
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -716,7 +716,7 @@
     </row>
     <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" s="24"/>
       <c r="C2" s="24"/>
@@ -762,13 +762,13 @@
       <c r="A4" s="7"/>
       <c r="B4" s="7"/>
       <c r="C4" s="21" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="D4" s="22" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="E4" s="23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="8"/>
@@ -780,25 +780,25 @@
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F5" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="H5" s="10" t="s">
+      <c r="I5" s="10" t="s">
         <v>14</v>
-      </c>
-      <c r="I5" s="10" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.2">
@@ -809,36 +809,36 @@
         <v>3</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D6" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="F6" s="12" t="s">
         <v>22</v>
-      </c>
-      <c r="F6" s="12" t="s">
-        <v>23</v>
       </c>
       <c r="G6" s="13" t="s">
         <v>6</v>
       </c>
       <c r="H6" s="13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I6" s="13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" s="15">
         <v>16</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D7" s="18"/>
       <c r="E7" s="18"/>
@@ -851,13 +851,13 @@
     </row>
     <row r="8" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" s="15">
         <v>16</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D8" s="18"/>
       <c r="E8" s="18"/>
@@ -870,27 +870,27 @@
     </row>
     <row r="9" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B9" s="15">
         <v>15</v>
       </c>
       <c r="C9" s="18"/>
       <c r="D9" s="18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G9" s="19"/>
       <c r="H9" s="19" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I9" s="19" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Uploaded 10-May-2021 11:29:08 {/src/main/resources/com/wakandaspace/drools_price_model/premiumCalculation.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/wakandaspace/drools_price_model/premiumCalculation.xlsx
+++ b/src/main/resources/com/wakandaspace/drools_price_model/premiumCalculation.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IBISDIALLO\Desktop\Reliance Models Pricing\Reliance Models Pricing\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="921"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="921"/>
   </bookViews>
   <sheets>
     <sheet name="Tariff" sheetId="1" r:id="rId1"/>
@@ -237,11 +242,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -387,6 +389,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -434,7 +439,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -469,7 +474,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -680,224 +685,220 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="40.42578125" style="16"/>
-    <col min="2" max="2" width="10.5703125" style="16"/>
-    <col min="3" max="6" width="25.140625" style="16" customWidth="1"/>
-    <col min="7" max="7" width="25.5703125" style="17" customWidth="1"/>
-    <col min="8" max="8" width="30.85546875" style="17" customWidth="1"/>
-    <col min="9" max="9" width="31.7109375" style="17" customWidth="1"/>
-    <col min="10" max="10" width="18.28515625" style="2"/>
-    <col min="11" max="11" width="10.7109375" style="2"/>
-    <col min="12" max="12" width="19" style="2"/>
-    <col min="13" max="1028" width="10.7109375" style="2"/>
-    <col min="1029" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="40.42578125" style="15"/>
+    <col min="2" max="2" width="10.5703125" style="15"/>
+    <col min="3" max="6" width="25.140625" style="15" customWidth="1"/>
+    <col min="7" max="7" width="25.5703125" style="16" customWidth="1"/>
+    <col min="8" max="8" width="30.85546875" style="16" customWidth="1"/>
+    <col min="9" max="9" width="31.7109375" style="16" customWidth="1"/>
+    <col min="10" max="10" width="18.28515625" style="1"/>
+    <col min="11" max="11" width="10.7109375" style="1"/>
+    <col min="12" max="12" width="19" style="1"/>
+    <col min="13" max="1028" width="10.7109375" style="1"/>
+    <col min="1029" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
     </row>
     <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="M2" s="3"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="M2" s="2"/>
     </row>
     <row r="3" spans="1:13" ht="14.1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="M3" s="3"/>
+      <c r="M3" s="2"/>
     </row>
     <row r="4" spans="1:13" ht="25.5" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="21" t="s">
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="22" t="s">
+      <c r="D4" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="23" t="s">
+      <c r="E4" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="21"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="M4" s="3"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="M4" s="2"/>
     </row>
     <row r="5" spans="1:13" ht="63.75" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="9" t="s">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F5" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="10" t="s">
+      <c r="G5" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="H5" s="10" t="s">
+      <c r="H5" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="I5" s="10" t="s">
+      <c r="I5" s="9" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="E6" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="F6" s="12" t="s">
+      <c r="F6" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="G6" s="13" t="s">
+      <c r="G6" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="H6" s="13" t="s">
+      <c r="H6" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="I6" s="13" t="s">
+      <c r="I6" s="12" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="15">
+      <c r="B7" s="14">
         <v>16</v>
       </c>
-      <c r="C7" s="18" t="s">
+      <c r="C7" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="19">
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="18">
         <v>0.91200000000000003</v>
       </c>
-      <c r="H7" s="19"/>
-      <c r="I7" s="19"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
     </row>
     <row r="8" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="15">
+      <c r="B8" s="14">
         <v>16</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="19">
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="18">
         <v>1</v>
       </c>
-      <c r="H8" s="19"/>
-      <c r="I8" s="19"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="18"/>
     </row>
     <row r="9" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="15">
+      <c r="B9" s="14">
         <v>15</v>
       </c>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18" t="s">
+      <c r="C9" s="17"/>
+      <c r="D9" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="18" t="s">
+      <c r="E9" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="18" t="s">
+      <c r="F9" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="G9" s="19"/>
-      <c r="H9" s="19" t="s">
+      <c r="G9" s="18"/>
+      <c r="H9" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="I9" s="19" t="s">
+      <c r="I9" s="18" t="s">
         <v>9</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B1:G1"/>
-    <mergeCell ref="A2:G2"/>
-  </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" r:id="rId1"/>
   <headerFooter>

</xml_diff>

<commit_message>
Uploaded 10-May-2021 11:33:40 {/src/main/resources/com/wakandaspace/drools_price_model/premiumCalculation.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/wakandaspace/drools_price_model/premiumCalculation.xlsx
+++ b/src/main/resources/com/wakandaspace/drools_price_model/premiumCalculation.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="26">
   <si>
     <t>RuleSet</t>
   </si>
@@ -242,7 +242,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -302,14 +302,17 @@
     <xf numFmtId="10" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="10" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="10" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -686,7 +689,7 @@
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C4" sqref="C4:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -705,30 +708,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
       <c r="H1" s="19"/>
       <c r="I1" s="19"/>
     </row>
     <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
       <c r="H2" s="19"/>
       <c r="I2" s="19"/>
       <c r="M2" s="2"/>
@@ -766,13 +769,11 @@
     <row r="4" spans="1:13" ht="25.5" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
-      <c r="C4" s="20" t="s">
+      <c r="C4" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" s="22" t="s">
+      <c r="D4" s="24"/>
+      <c r="E4" s="21" t="s">
         <v>24</v>
       </c>
       <c r="F4" s="20"/>
@@ -899,6 +900,9 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C4:D4"/>
+  </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" r:id="rId1"/>
   <headerFooter>

</xml_diff>

<commit_message>
Uploaded 11-May-2021 12:53:24 {/src/main/resources/com/wakandaspace/drools_price_model/premiumCalculation.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/wakandaspace/drools_price_model/premiumCalculation.xlsx
+++ b/src/main/resources/com/wakandaspace/drools_price_model/premiumCalculation.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IBISDIALLO\Desktop\Reliance Models Pricing\Reliance Models Pricing\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="921"/>
   </bookViews>
@@ -83,9 +78,6 @@
     <t>premiumCalculation</t>
   </si>
   <si>
-    <t>getPreAuthorizationRequired().equals("$param")</t>
-  </si>
-  <si>
     <t>plan</t>
   </si>
   <si>
@@ -102,6 +94,9 @@
   </si>
   <si>
     <t>$plan: Plan</t>
+  </si>
+  <si>
+    <t>getPreAuthorizationRequired()</t>
   </si>
 </sst>
 </file>
@@ -442,7 +437,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -477,7 +472,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -689,14 +684,15 @@
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:D4"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="40.42578125" style="15"/>
     <col min="2" max="2" width="10.5703125" style="15"/>
-    <col min="3" max="6" width="25.140625" style="15" customWidth="1"/>
+    <col min="3" max="3" width="26" style="15" customWidth="1"/>
+    <col min="4" max="6" width="25.140625" style="15" customWidth="1"/>
     <col min="7" max="7" width="25.5703125" style="16" customWidth="1"/>
     <col min="8" max="8" width="30.85546875" style="16" customWidth="1"/>
     <col min="9" max="9" width="31.7109375" style="16" customWidth="1"/>
@@ -770,11 +766,11 @@
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
       <c r="C4" s="23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D4" s="24"/>
       <c r="E4" s="21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F4" s="20"/>
       <c r="G4" s="7"/>
@@ -782,11 +778,11 @@
       <c r="I4" s="7"/>
       <c r="M4" s="2"/>
     </row>
-    <row r="5" spans="1:13" ht="63.75" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" ht="26.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="8" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>9</v>
@@ -818,22 +814,22 @@
         <v>10</v>
       </c>
       <c r="D6" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="F6" s="11" t="s">
         <v>21</v>
-      </c>
-      <c r="F6" s="11" t="s">
-        <v>22</v>
       </c>
       <c r="G6" s="12" t="s">
         <v>6</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I6" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Uploaded 11-May-2021 13:01:36 {/src/main/resources/com/wakandaspace/drools_price_model/premiumCalculation.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/wakandaspace/drools_price_model/premiumCalculation.xlsx
+++ b/src/main/resources/com/wakandaspace/drools_price_model/premiumCalculation.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="26">
   <si>
     <t>RuleSet</t>
   </si>
@@ -237,7 +237,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -249,9 +249,6 @@
     <xf numFmtId="10" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -307,6 +304,15 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -683,19 +689,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="F2" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="40.42578125" style="15"/>
-    <col min="2" max="2" width="10.5703125" style="15"/>
-    <col min="3" max="3" width="26" style="15" customWidth="1"/>
-    <col min="4" max="6" width="25.140625" style="15" customWidth="1"/>
-    <col min="7" max="7" width="25.5703125" style="16" customWidth="1"/>
-    <col min="8" max="8" width="30.85546875" style="16" customWidth="1"/>
-    <col min="9" max="9" width="31.7109375" style="16" customWidth="1"/>
+    <col min="1" max="1" width="40.42578125" style="14"/>
+    <col min="2" max="2" width="10.5703125" style="14"/>
+    <col min="3" max="3" width="26" style="14" customWidth="1"/>
+    <col min="4" max="6" width="25.140625" style="14" customWidth="1"/>
+    <col min="7" max="7" width="25.5703125" style="15" customWidth="1"/>
+    <col min="8" max="8" width="30.85546875" style="15" customWidth="1"/>
+    <col min="9" max="9" width="31.7109375" style="15" customWidth="1"/>
     <col min="10" max="10" width="18.28515625" style="1"/>
     <col min="11" max="11" width="10.7109375" style="1"/>
     <col min="12" max="12" width="19" style="1"/>
@@ -704,32 +710,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
     </row>
     <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
       <c r="M2" s="2"/>
     </row>
     <row r="3" spans="1:13" ht="14.1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
@@ -751,153 +757,150 @@
       <c r="F3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>5</v>
-      </c>
+      <c r="H3" s="25"/>
+      <c r="I3" s="26"/>
       <c r="M3" s="2"/>
     </row>
     <row r="4" spans="1:13" ht="25.5" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="6"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="23" t="s">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="24"/>
-      <c r="E4" s="21" t="s">
+      <c r="D4" s="23"/>
+      <c r="E4" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="20"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
       <c r="M4" s="2"/>
     </row>
     <row r="5" spans="1:13" ht="26.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="8" t="s">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="G5" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="H5" s="9" t="s">
+      <c r="H5" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="I5" s="9" t="s">
+      <c r="I5" s="8" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="E6" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="F6" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="G6" s="12" t="s">
+      <c r="G6" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="H6" s="12" t="s">
+      <c r="H6" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="I6" s="12" t="s">
+      <c r="I6" s="11" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="14">
+      <c r="B7" s="13">
         <v>16</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="18">
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="17">
         <v>0.91200000000000003</v>
       </c>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="17"/>
     </row>
     <row r="8" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="14">
+      <c r="B8" s="13">
         <v>16</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="18">
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="17">
         <v>1</v>
       </c>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
     </row>
     <row r="9" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="14">
+      <c r="B9" s="13">
         <v>15</v>
       </c>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17" t="s">
+      <c r="C9" s="16"/>
+      <c r="D9" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="17" t="s">
+      <c r="E9" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="17" t="s">
+      <c r="F9" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18" t="s">
+      <c r="G9" s="17"/>
+      <c r="H9" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="I9" s="18" t="s">
+      <c r="I9" s="17" t="s">
         <v>9</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="C4:D4"/>
+    <mergeCell ref="G3:I3"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" r:id="rId1"/>

</xml_diff>